<commit_message>
Added files of Dead and Missing and updated quality assurance document
</commit_message>
<xml_diff>
--- a/delegation.xlsx
+++ b/delegation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
   <si>
     <t>Column1</t>
   </si>
@@ -241,19 +241,43 @@
     <t>Data Dictionary</t>
   </si>
   <si>
-    <t>What to search</t>
-  </si>
-  <si>
-    <t>Advisory form of NDRRMC for typhoon, earthquake, volcanic eruption and tsunami</t>
-  </si>
-  <si>
-    <t>Supplies needed for each and every disasters</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
     <t>Not yet final</t>
+  </si>
+  <si>
+    <t>Delegation: 2/15/2017</t>
+  </si>
+  <si>
+    <t>Look for BI tool and on thursday we'll decide which one to use</t>
+  </si>
+  <si>
+    <t>Learn ETL</t>
+  </si>
+  <si>
+    <t>Continue working on Quality Assurance Document</t>
+  </si>
+  <si>
+    <t>Install Ubuntu and Cassandra on Virtual Machine</t>
+  </si>
+  <si>
+    <t>Explore Cassandra</t>
+  </si>
+  <si>
+    <t>Agenda on Thursday: 2/14/2017</t>
+  </si>
+  <si>
+    <t>Choose BI Tool</t>
+  </si>
+  <si>
+    <t>Finalize DFD</t>
+  </si>
+  <si>
+    <t>Finalize ERD</t>
+  </si>
+  <si>
+    <t>Come up with a step by step process on how to use the system.</t>
   </si>
 </sst>
 </file>
@@ -315,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -403,127 +427,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -538,32 +448,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -868,13 +764,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +811,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -942,7 +839,9 @@
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -971,7 +870,9 @@
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -1098,7 +999,9 @@
       <c r="B25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
@@ -1162,7 +1065,9 @@
       <c r="B33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="9"/>
+      <c r="C33" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
@@ -1196,7 +1101,9 @@
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="9"/>
+      <c r="C37" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
@@ -1296,7 +1203,9 @@
       <c r="B49" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="9"/>
+      <c r="C49" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
@@ -1323,7 +1232,9 @@
       <c r="B52" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="9"/>
+      <c r="C52" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -1365,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,10 +1298,8 @@
       <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="23"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1400,12 +1309,10 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="17"/>
+        <v>73</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1415,10 +1322,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1428,7 +1335,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1438,10 +1345,10 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1451,22 +1358,20 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1484,7 +1389,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1503,7 +1408,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,7 +1416,7 @@
         <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1530,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1557,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,14 +1473,81 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>77</v>
       </c>
+      <c r="B24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="17"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="17"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E2:F4"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="E1:F1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="B1">
     <cfRule type="cellIs" priority="3" operator="equal">

</xml_diff>